<commit_message>
added new data for Policia
</commit_message>
<xml_diff>
--- a/data/Negociado_de_Policia/npprDS_ofensores.xlsx
+++ b/data/Negociado_de_Policia/npprDS_ofensores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Negociado_de_Policia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FED26A-9F90-476A-BE84-AF1FD298305C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EECE46B-B728-4A32-93A0-9F12FB635B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="1404" windowWidth="17280" windowHeight="9420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="15" r:id="rId1"/>
@@ -416,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1570,7 +1570,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1593,10 +1595,10 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1604,10 +1606,10 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1615,10 +1617,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1626,10 +1628,10 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1637,10 +1639,10 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1648,10 +1650,10 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1659,10 +1661,10 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1670,10 +1672,10 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1681,10 +1683,10 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1692,10 +1694,10 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1703,10 +1705,10 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1714,10 +1716,10 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1725,10 +1727,10 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1736,10 +1738,10 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>9</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1747,10 +1749,10 @@
         <v>11</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="C16">
-        <v>30</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>